<commit_message>
added unitname, matrixname for both fieldresults and habitatresults.
Also created a csv file that contains sheets to both field/habitat results
</commit_message>
<xml_diff>
--- a/RelationshipMap.xlsx
+++ b/RelationshipMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toled\Desktop\SCCWRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDC1531-D7AE-48BD-A692-50496318FF5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C599F1-8B05-4E95-ABD3-5F4944ED6019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="3060" windowWidth="19230" windowHeight="11100" xr2:uid="{F9812EE0-3961-FE4F-824E-79A3DFBA05C9}"/>
+    <workbookView xWindow="57300" yWindow="885" windowWidth="23160" windowHeight="11910" activeTab="1" xr2:uid="{F9812EE0-3961-FE4F-824E-79A3DFBA05C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Analytes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="190">
   <si>
     <t>Temperature</t>
   </si>
@@ -601,6 +601,9 @@
   </si>
   <si>
     <t>EvidenceOfFires</t>
+  </si>
+  <si>
+    <t>FieldResult</t>
   </si>
 </sst>
 </file>
@@ -994,11 +997,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71EBA9C-90F2-5945-896F-0A96C8D71702}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
@@ -1009,7 +1012,7 @@
     <col min="7" max="7" width="69.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -1147,7 +1150,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>172</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>173</v>
       </c>
@@ -1262,7 +1265,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>187</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>176</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>175</v>
       </c>
@@ -1351,7 +1354,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>179</v>
       </c>
@@ -1420,7 +1423,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>180</v>
       </c>
@@ -1443,7 +1446,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>181</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>182</v>
       </c>
@@ -1489,7 +1492,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>183</v>
       </c>
@@ -1512,7 +1515,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>184</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>185</v>
       </c>
@@ -1558,7 +1561,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>186</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1650,7 +1653,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1673,7 +1676,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>188</v>
       </c>
@@ -1788,7 +1791,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -1834,7 +1837,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -1857,7 +1860,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -1890,11 +1893,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227F44FB-EC10-E34D-B181-672CA1B29D12}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.125" bestFit="1" customWidth="1"/>
@@ -1906,7 +1909,7 @@
     <col min="12" max="12" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1923,7 +1926,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1934,7 +1937,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1945,7 +1948,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1956,7 +1959,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1967,7 +1970,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -1978,7 +1981,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1989,7 +1992,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2011,7 +2014,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -2022,7 +2025,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -2033,7 +2036,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -2044,7 +2047,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>177</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -2072,7 +2075,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -2083,7 +2086,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -2105,7 +2108,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>159</v>
       </c>
@@ -2116,7 +2119,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -2138,7 +2141,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -2160,7 +2163,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -2171,7 +2174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -2182,7 +2185,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>89</v>
       </c>
@@ -2193,7 +2196,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>152</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>152</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>152</v>
       </c>
@@ -2235,7 +2238,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>152</v>
       </c>
@@ -2246,10 +2249,10 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>154</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>155</v>
       </c>
@@ -2291,7 +2294,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>161</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>162</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>90</v>
       </c>
@@ -2328,7 +2331,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>91</v>
       </c>
@@ -2339,7 +2342,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>92</v>
       </c>
@@ -2350,7 +2353,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>93</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -2372,7 +2375,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -2394,7 +2397,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -2405,7 +2408,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -2427,7 +2430,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>99</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -2449,7 +2452,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -2460,7 +2463,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -2471,7 +2474,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
         <v>106</v>
       </c>
@@ -2482,7 +2485,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -2496,7 +2499,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -2510,7 +2513,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
         <v>112</v>
       </c>
@@ -2521,7 +2524,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -2532,7 +2535,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
         <v>116</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
         <v>117</v>
       </c>
@@ -2571,7 +2574,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -2582,7 +2585,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
         <v>122</v>
       </c>
@@ -2593,7 +2596,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
         <v>123</v>
       </c>
@@ -2604,7 +2607,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
         <v>124</v>
       </c>
@@ -2615,7 +2618,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A61" t="s">
         <v>125</v>
       </c>
@@ -2626,7 +2629,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
         <v>126</v>
       </c>
@@ -2637,7 +2640,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
         <v>128</v>
       </c>
@@ -2648,7 +2651,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
         <v>129</v>
       </c>
@@ -2659,7 +2662,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
         <v>165</v>
       </c>
@@ -2670,7 +2673,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
         <v>166</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
almost done adding in the units for each analyte. added the remaining columns except device names
</commit_message>
<xml_diff>
--- a/RelationshipMap.xlsx
+++ b/RelationshipMap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toled\Desktop\SCCWRP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toled\Desktop\BLM_data_reformatter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C599F1-8B05-4E95-ABD3-5F4944ED6019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FD4A34-35A9-4C3F-8042-AF4484C2C18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57300" yWindow="885" windowWidth="23160" windowHeight="11910" activeTab="1" xr2:uid="{F9812EE0-3961-FE4F-824E-79A3DFBA05C9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{F9812EE0-3961-FE4F-824E-79A3DFBA05C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Analytes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="190">
   <si>
     <t>Temperature</t>
   </si>
@@ -1891,10 +1891,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227F44FB-EC10-E34D-B181-672CA1B29D12}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="B59" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2695,6 +2695,54 @@
         <v>24</v>
       </c>
     </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D68" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A69" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A71" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A72" t="s">
+        <v>140</v>
+      </c>
+      <c r="D72" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A73" t="s">
+        <v>139</v>
+      </c>
+      <c r="D73" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>